<commit_message>
added the metadata fields and updated resulted tables
added description and keywords
</commit_message>
<xml_diff>
--- a/results/metadata.xlsx
+++ b/results/metadata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Title</t>
+          <t>- Title</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Creator (Author)</t>
+          <t>- Creator (Author)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>John Doove</t>
+          <t>John Doove, Germaine Poot, Karin van Grieken, Gül Akcaova</t>
         </is>
       </c>
     </row>
@@ -492,7 +492,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>- Date</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>- Description</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Programma</t>
+          <t>The text describes the ambitions and initiatives related to open science and research information in the Netherlands, particularly in the context of higher education institutions (hbo). It mentions projects, platforms, and collaborations aimed at making research information open, accessible, and visible. It also discusses the role of SURF (a collaborative organization for ICT in Dutch education and research) in facilitating open science in hbo.</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Identifier (DOI)</t>
+          <t>- Keywords</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>None provided</t>
+          <t>Open science, onderzoeksinformatie, ambitie, hogescholen, SURF, project, NPPO, Knowledge Exchange, Persistent Identifiers, ORCID, roadmap</t>
         </is>
       </c>
     </row>
@@ -543,12 +543,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Publisher</t>
+          <t>- Type</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SURF</t>
+          <t>Text (document, article)</t>
         </is>
       </c>
     </row>
@@ -560,12 +560,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rights</t>
+          <t>- Identifier (DOI)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>No specific rights information provided</t>
+          <t>No DOI provided</t>
         </is>
       </c>
     </row>
@@ -577,12 +577,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>- Publisher</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Dutch</t>
+          <t>No specific publisher mentioned</t>
         </is>
       </c>
     </row>
@@ -594,12 +594,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>- Rights</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>No specific format mentioned</t>
+          <t>No specific rights mentioned</t>
         </is>
       </c>
     </row>
@@ -611,12 +611,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Source</t>
+          <t>- Language</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>No specific source mentioned</t>
+          <t>Dutch</t>
         </is>
       </c>
     </row>
@@ -628,12 +628,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Relation</t>
+          <t>- Format</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>No specific relation mentioned</t>
+          <t>Textual format (possibly in a digital document)</t>
         </is>
       </c>
     </row>
@@ -645,12 +645,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Coverage</t>
+          <t>- Source</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>No specific coverage mentioned</t>
+          <t>No specific source mentioned</t>
         </is>
       </c>
     </row>
@@ -662,12 +662,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Title</t>
+          <t>- Relation</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Open science en onderzoeksinformatie</t>
+          <t>Various projects and collaborations are mentioned, such as the relation between the Open Science and onderzoeksinformatie project and the NPPO project, and the relation between SURF and the "Adviescollege Open Science in het hbo" of the Vereniging Hogescholen.</t>
         </is>
       </c>
     </row>
@@ -679,12 +679,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Creator (Author)</t>
+          <t>- Coverage</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>John Doove</t>
+          <t>The text primarily focuses on open science and research information initiatives in the Netherlands, particularly in hbo (higher education). It also mentions European collaborations through Knowledge Exchange.</t>
         </is>
       </c>
     </row>
@@ -696,12 +696,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>- Title</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>No specific date mentioned</t>
+          <t>Open science en onderzoeksinformatie</t>
         </is>
       </c>
     </row>
@@ -713,12 +713,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>- Creator (Author)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Programma</t>
+          <t>John Doove, Germaine Poot, Karin van Grieken, Gül Akcaova</t>
         </is>
       </c>
     </row>
@@ -730,12 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Identifier (DOI)</t>
+          <t>- Date</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>None provided</t>
+          <t>No specific date mentioned</t>
         </is>
       </c>
     </row>
@@ -747,12 +747,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Publisher</t>
+          <t>- Description</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>SURF</t>
+          <t>The text describes the ambitions and initiatives related to open science and research information in the Netherlands, particularly in the context of higher education institutions (hbo). It mentions projects, platforms, and collaborations aimed at making research information open, accessible, and visible. It also discusses the role of SURF (a collaborative organization for ICT in Dutch education and research) in facilitating open science in hbo.</t>
         </is>
       </c>
     </row>
@@ -764,12 +764,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Rights</t>
+          <t>- Keywords</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>No specific rights information provided</t>
+          <t>Open science, onderzoeksinformatie, ambitie, hogescholen, SURF, project, NPPO, Knowledge Exchange, Persistent Identifiers, ORCID, roadmap</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>- Type</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Dutch</t>
+          <t>Text (document, article)</t>
         </is>
       </c>
     </row>
@@ -798,12 +798,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>- Identifier (DOI)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>No specific format mentioned</t>
+          <t>No DOI provided</t>
         </is>
       </c>
     </row>
@@ -815,12 +815,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Source</t>
+          <t>- Publisher</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>No specific source mentioned</t>
+          <t>No specific publisher mentioned</t>
         </is>
       </c>
     </row>
@@ -832,12 +832,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Relation</t>
+          <t>- Rights</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>No specific relation mentioned</t>
+          <t>No specific rights mentioned</t>
         </is>
       </c>
     </row>
@@ -849,12 +849,80 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Coverage</t>
+          <t>- Language</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>No specific coverage mentioned</t>
+          <t>Dutch</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>KRTINN-Openscienceenonderzoeksinformatie-060923-1508-1296.pdf</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>- Format</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Textual format (possibly in a digital document)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>KRTINN-Openscienceenonderzoeksinformatie-060923-1508-1296.pdf</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>- Source</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>No specific source mentioned</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>KRTINN-Openscienceenonderzoeksinformatie-060923-1508-1296.pdf</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>- Relation</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Various projects and collaborations are mentioned, such as the relation between the Open Science and onderzoeksinformatie project and the NPPO project, and the relation between SURF and the "Adviescollege Open Science in het hbo" of the Vereniging Hogescholen.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>KRTINN-Openscienceenonderzoeksinformatie-060923-1508-1296.pdf</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>- Coverage</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>The text primarily focuses on open science and research information initiatives in the Netherlands, particularly in hbo (higher education). It also mentions European collaborations through Knowledge Exchange.</t>
         </is>
       </c>
     </row>

</xml_diff>